<commit_message>
cleaned up graph ready for printing
</commit_message>
<xml_diff>
--- a/correcting_gradient_values.xlsx
+++ b/correcting_gradient_values.xlsx
@@ -661,7 +661,68 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Plot showing the effect of the</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> formula adjusting raw angles calculated using the arduino for a systematic error.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -701,6 +762,46 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="0.5"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
           <c:xVal>
             <c:numRef>
               <c:f>Sheet1!$A$3:$A$12</c:f>
@@ -1085,6 +1186,8 @@
         <c:axId val="347718824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="50"/>
+          <c:min val="-5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -1355,6 +1458,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2865,7 +2972,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>